<commit_message>
Added logos to Allsvenskan2001.xlsx
</commit_message>
<xml_diff>
--- a/EPPlus.WebSampleMvc.NetCore/data/Allsvenskan2001.xlsx
+++ b/EPPlus.WebSampleMvc.NetCore/data/Allsvenskan2001.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mats\dev\EPPlusSoftware\EPPlus6.WebSamples\EPPlus.WebSampleMvc.NetCore\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mats\dev\EPPlusSoftware\EPPlus.WebSamples\EPPlus.WebSampleMvc.NetCore\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D43862D-6288-44B8-BCCE-0DBB53F95C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865597EE-B505-408A-B720-1F4F7B27A8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CC10EFD2-A4CF-4F7B-8E25-A2032FB846DE}"/>
+    <workbookView xWindow="95880" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CC10EFD2-A4CF-4F7B-8E25-A2032FB846DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -585,179 +585,209 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -784,6 +814,854 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>609600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A474E74B-40F8-480A-BDB2-C973073F76B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="866775" y="1657350"/>
+          <a:ext cx="257175" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{685320DD-2012-4752-AB98-1A73338E66D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="885826" y="2276476"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8490777C-67E5-4BC6-A743-DE90339D0620}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="876301" y="2533651"/>
+          <a:ext cx="247650" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B9EA950-972F-4E04-8855-5AA5BE8A34C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="895350" y="2800350"/>
+          <a:ext cx="219075" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>533400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{119B6688-58AA-4A75-8544-C5F5F4F4DE10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="904875" y="3333750"/>
+          <a:ext cx="209550" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>247651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AA34F0F-D8CC-4C50-A783-B084A8974154}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="904876" y="4105276"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8063D6F-D000-43C3-97EF-A5E3E88AE2B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="904875" y="4381500"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71DFADCF-FBFE-4A98-BE14-FE420E625E74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="895350" y="4657725"/>
+          <a:ext cx="238125" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BC702A6-2941-47ED-9916-19C2CEA180D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="904875" y="4905375"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD51C384-F21C-46F9-8BD9-E125D89747C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="904875" y="5143500"/>
+          <a:ext cx="219075" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D54F14BB-3B5E-4B6C-A733-40664626BB72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="904875" y="5553075"/>
+          <a:ext cx="238125" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E824AA7C-31F2-4BDB-9F21-F478E9D4CB2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="895350" y="5972175"/>
+          <a:ext cx="257175" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE45C00-86C8-433F-8473-019B6793BA4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="904875" y="6238875"/>
+          <a:ext cx="228600" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84769677-7E2B-4606-AA34-B2812F9E5B9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="904875" y="3886200"/>
+          <a:ext cx="200025" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1083,649 +1961,676 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047A5EC2-D577-486C-8E0D-C6229686D238}">
-  <dimension ref="B1:M21"/>
+  <dimension ref="B1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="6.54296875" customWidth="1"/>
-    <col min="2" max="2" width="5.2265625" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="6" width="5.6796875" customWidth="1"/>
-    <col min="7" max="7" width="5.7265625" customWidth="1"/>
-    <col min="8" max="8" width="3.86328125" customWidth="1"/>
-    <col min="9" max="9" width="2.1796875" customWidth="1"/>
-    <col min="10" max="10" width="3.86328125" customWidth="1"/>
-    <col min="11" max="12" width="5.7265625" customWidth="1"/>
-    <col min="13" max="13" width="13.08984375" customWidth="1"/>
+    <col min="2" max="3" width="5.2265625" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" customWidth="1"/>
+    <col min="5" max="7" width="5.6796875" customWidth="1"/>
+    <col min="8" max="8" width="5.7265625" customWidth="1"/>
+    <col min="9" max="9" width="3.86328125" customWidth="1"/>
+    <col min="10" max="10" width="2.1796875" customWidth="1"/>
+    <col min="11" max="11" width="3.86328125" customWidth="1"/>
+    <col min="12" max="13" width="5.7265625" customWidth="1"/>
+    <col min="14" max="14" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="21" x14ac:dyDescent="1">
+    <row r="1" spans="2:22" ht="21" x14ac:dyDescent="1">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.75">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.75">
       <c r="B3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="21.75" thickBot="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="D4" s="1"/>
+    <row r="4" spans="2:22" ht="21.75" thickBot="1" x14ac:dyDescent="1.1499999999999999">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:13" s="2" customFormat="1" ht="30.25" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27" t="s">
+    <row r="5" spans="2:22" s="2" customFormat="1" ht="30.25" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B5" s="23"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="E5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="F5" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="G5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="H5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="I5" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="28" t="s">
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="M5" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="N5" s="14" t="s">
         <v>18</v>
       </c>
+      <c r="Q5"/>
     </row>
-    <row r="6" spans="2:13" s="2" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
-      <c r="B6" s="60">
+    <row r="6" spans="2:22" s="2" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
+      <c r="B6" s="56">
         <v>1</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="71"/>
+      <c r="D6" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="60">
+      <c r="E6" s="56">
         <v>26</v>
       </c>
-      <c r="E6" s="60">
+      <c r="F6" s="56">
         <v>14</v>
       </c>
-      <c r="F6" s="60">
+      <c r="G6" s="56">
         <v>6</v>
       </c>
-      <c r="G6" s="60">
+      <c r="H6" s="56">
         <v>6</v>
       </c>
-      <c r="H6" s="62">
+      <c r="I6" s="58">
         <v>45</v>
       </c>
-      <c r="I6" s="63" t="s">
+      <c r="J6" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="64">
+      <c r="K6" s="60">
         <v>28</v>
       </c>
-      <c r="K6" s="60">
-        <f>H6-J6</f>
+      <c r="L6" s="56">
+        <f>I6-K6</f>
         <v>17</v>
       </c>
-      <c r="L6" s="65">
-        <f>E6*3+F6</f>
+      <c r="M6" s="61">
+        <f>F6*3+G6</f>
         <v>48</v>
       </c>
-      <c r="M6" s="66" t="s">
+      <c r="N6" s="62" t="s">
         <v>25</v>
       </c>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
     </row>
-    <row r="7" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B7" s="30">
+    <row r="7" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B7" s="26">
         <v>2</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="72"/>
+      <c r="D7" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="30">
+      <c r="E7" s="26">
         <v>26</v>
       </c>
-      <c r="E7" s="30">
+      <c r="F7" s="26">
         <v>13</v>
       </c>
-      <c r="F7" s="30">
+      <c r="G7" s="26">
         <v>8</v>
       </c>
-      <c r="G7" s="30">
+      <c r="H7" s="26">
         <v>5</v>
       </c>
-      <c r="H7" s="32">
+      <c r="I7" s="28">
         <v>36</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="J7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="34">
+      <c r="K7" s="30">
         <v>24</v>
       </c>
-      <c r="K7" s="30">
-        <f t="shared" ref="K7:K21" si="0">H7-J7</f>
+      <c r="L7" s="26">
+        <f t="shared" ref="L7:L19" si="0">I7-K7</f>
         <v>12</v>
       </c>
-      <c r="L7" s="35">
-        <f t="shared" ref="L7:L21" si="1">E7*3+F7</f>
+      <c r="M7" s="31">
+        <f t="shared" ref="M7:M19" si="1">F7*3+G7</f>
         <v>47</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="N7" s="81" t="s">
         <v>26</v>
       </c>
+      <c r="S7"/>
+      <c r="T7"/>
     </row>
-    <row r="8" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="36">
+    <row r="8" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B8" s="32">
         <v>3</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="36">
+      <c r="E8" s="32">
         <v>26</v>
       </c>
-      <c r="E8" s="36">
+      <c r="F8" s="32">
         <v>12</v>
       </c>
-      <c r="F8" s="36">
+      <c r="G8" s="32">
         <v>9</v>
       </c>
-      <c r="G8" s="36">
+      <c r="H8" s="32">
         <v>5</v>
       </c>
-      <c r="H8" s="38">
+      <c r="I8" s="34">
         <v>45</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="J8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="40">
+      <c r="K8" s="36">
         <v>29</v>
       </c>
-      <c r="K8" s="36">
+      <c r="L8" s="32">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="L8" s="41">
+      <c r="M8" s="37">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="M8" s="16"/>
+      <c r="N8" s="81"/>
     </row>
-    <row r="9" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B9" s="36">
+    <row r="9" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B9" s="32">
         <v>4</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="73"/>
+      <c r="D9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="36">
+      <c r="E9" s="32">
         <v>26</v>
       </c>
-      <c r="E9" s="36">
+      <c r="F9" s="32">
         <v>12</v>
       </c>
-      <c r="F9" s="36">
+      <c r="G9" s="32">
         <v>8</v>
       </c>
-      <c r="G9" s="36">
+      <c r="H9" s="32">
         <v>6</v>
       </c>
-      <c r="H9" s="38">
+      <c r="I9" s="34">
         <v>41</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="J9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="40">
+      <c r="K9" s="36">
         <v>31</v>
       </c>
-      <c r="K9" s="36">
+      <c r="L9" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L9" s="41">
+      <c r="M9" s="37">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="M9" s="16"/>
+      <c r="N9" s="81"/>
     </row>
-    <row r="10" spans="2:13" s="2" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B10" s="42">
+    <row r="10" spans="2:22" s="2" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B10" s="38">
         <v>5</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="74"/>
+      <c r="D10" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="42">
+      <c r="E10" s="38">
         <v>26</v>
       </c>
-      <c r="E10" s="42">
+      <c r="F10" s="38">
         <v>11</v>
       </c>
-      <c r="F10" s="42">
+      <c r="G10" s="38">
         <v>9</v>
       </c>
-      <c r="G10" s="42">
+      <c r="H10" s="38">
         <v>6</v>
       </c>
-      <c r="H10" s="44">
+      <c r="I10" s="40">
         <v>47</v>
       </c>
-      <c r="I10" s="45" t="s">
+      <c r="J10" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="46">
+      <c r="K10" s="42">
         <v>29</v>
       </c>
-      <c r="K10" s="42">
+      <c r="L10" s="38">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="L10" s="47">
+      <c r="M10" s="43">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="M10" s="17" t="s">
+      <c r="N10" s="16" t="s">
         <v>27</v>
       </c>
+      <c r="R10"/>
+      <c r="V10"/>
     </row>
-    <row r="11" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B11" s="48">
+    <row r="11" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B11" s="44">
         <v>6</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="75"/>
+      <c r="D11" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="48">
+      <c r="E11" s="44">
         <v>26</v>
       </c>
-      <c r="E11" s="48">
+      <c r="F11" s="44">
         <v>10</v>
       </c>
-      <c r="F11" s="48">
+      <c r="G11" s="44">
         <v>9</v>
       </c>
-      <c r="G11" s="48">
+      <c r="H11" s="44">
         <v>7</v>
       </c>
-      <c r="H11" s="50">
+      <c r="I11" s="46">
         <v>36</v>
       </c>
-      <c r="I11" s="51" t="s">
+      <c r="J11" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="52">
+      <c r="K11" s="48">
         <v>33</v>
       </c>
-      <c r="K11" s="48">
+      <c r="L11" s="44">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L11" s="53">
+      <c r="M11" s="49">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
     </row>
-    <row r="12" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B12" s="48">
+    <row r="12" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B12" s="44">
         <v>7</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="75"/>
+      <c r="D12" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="48">
+      <c r="E12" s="44">
         <v>26</v>
       </c>
-      <c r="E12" s="48">
+      <c r="F12" s="44">
         <v>10</v>
       </c>
-      <c r="F12" s="48">
+      <c r="G12" s="44">
         <v>8</v>
       </c>
-      <c r="G12" s="48">
+      <c r="H12" s="44">
         <v>8</v>
       </c>
-      <c r="H12" s="50">
+      <c r="I12" s="46">
         <v>50</v>
       </c>
-      <c r="I12" s="51" t="s">
+      <c r="J12" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="52">
+      <c r="K12" s="48">
         <v>31</v>
       </c>
-      <c r="K12" s="48">
+      <c r="L12" s="44">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="L12" s="53">
+      <c r="M12" s="49">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
     </row>
-    <row r="13" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B13" s="48">
+    <row r="13" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B13" s="44">
         <v>8</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="75"/>
+      <c r="D13" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="48">
+      <c r="E13" s="44">
         <v>26</v>
       </c>
-      <c r="E13" s="48">
+      <c r="F13" s="44">
         <v>8</v>
       </c>
-      <c r="F13" s="48">
+      <c r="G13" s="44">
         <v>9</v>
       </c>
-      <c r="G13" s="48">
+      <c r="H13" s="44">
         <v>9</v>
       </c>
-      <c r="H13" s="50">
+      <c r="I13" s="46">
         <v>48</v>
       </c>
-      <c r="I13" s="51" t="s">
+      <c r="J13" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="52">
+      <c r="K13" s="48">
         <v>44</v>
       </c>
-      <c r="K13" s="48">
+      <c r="L13" s="44">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="L13" s="53">
+      <c r="M13" s="49">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
     </row>
-    <row r="14" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B14" s="48">
+    <row r="14" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B14" s="44">
         <v>9</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="75"/>
+      <c r="D14" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="48">
+      <c r="E14" s="44">
         <v>26</v>
       </c>
-      <c r="E14" s="48">
+      <c r="F14" s="44">
         <v>9</v>
       </c>
-      <c r="F14" s="48">
+      <c r="G14" s="44">
         <v>5</v>
       </c>
-      <c r="G14" s="48">
+      <c r="H14" s="44">
         <v>12</v>
       </c>
-      <c r="H14" s="50">
+      <c r="I14" s="46">
         <v>39</v>
       </c>
-      <c r="I14" s="51" t="s">
+      <c r="J14" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="52">
+      <c r="K14" s="48">
         <v>46</v>
       </c>
-      <c r="K14" s="48">
+      <c r="L14" s="44">
         <f t="shared" si="0"/>
         <v>-7</v>
       </c>
-      <c r="L14" s="53">
+      <c r="M14" s="49">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
     </row>
-    <row r="15" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B15" s="48">
+    <row r="15" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B15" s="44">
         <v>10</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="75"/>
+      <c r="D15" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="48">
+      <c r="E15" s="44">
         <v>26</v>
       </c>
-      <c r="E15" s="48">
+      <c r="F15" s="44">
         <v>9</v>
       </c>
-      <c r="F15" s="48">
+      <c r="G15" s="44">
         <v>3</v>
       </c>
-      <c r="G15" s="48">
+      <c r="H15" s="44">
         <v>14</v>
       </c>
-      <c r="H15" s="50">
+      <c r="I15" s="46">
         <v>31</v>
       </c>
-      <c r="I15" s="51" t="s">
+      <c r="J15" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="52">
+      <c r="K15" s="48">
         <v>51</v>
       </c>
-      <c r="K15" s="48">
+      <c r="L15" s="44">
         <f t="shared" si="0"/>
         <v>-20</v>
       </c>
-      <c r="L15" s="53">
+      <c r="M15" s="49">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
     </row>
-    <row r="16" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="16" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="B16" s="3">
         <v>11</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="76"/>
+      <c r="D16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>26</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
         <v>7</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
         <v>8</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>11</v>
       </c>
-      <c r="H16" s="11">
+      <c r="I16" s="11">
         <v>28</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J16" s="12">
+      <c r="K16" s="12">
         <v>37</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L16" s="3">
         <f t="shared" si="0"/>
         <v>-9</v>
       </c>
-      <c r="L16" s="13">
+      <c r="M16" s="13">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
     </row>
-    <row r="17" spans="2:13" s="2" customFormat="1" ht="45" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B17" s="67">
+    <row r="17" spans="2:14" s="2" customFormat="1" ht="45" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B17" s="63">
         <v>12</v>
       </c>
-      <c r="C17" s="68" t="s">
+      <c r="C17" s="77"/>
+      <c r="D17" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="67">
+      <c r="E17" s="63">
         <v>26</v>
       </c>
-      <c r="E17" s="67">
+      <c r="F17" s="63">
         <v>7</v>
       </c>
-      <c r="F17" s="67">
+      <c r="G17" s="63">
         <v>8</v>
       </c>
-      <c r="G17" s="67">
+      <c r="H17" s="63">
         <v>11</v>
       </c>
-      <c r="H17" s="69">
+      <c r="I17" s="65">
         <v>29</v>
       </c>
-      <c r="I17" s="70" t="s">
+      <c r="J17" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="J17" s="71">
+      <c r="K17" s="67">
         <v>40</v>
       </c>
-      <c r="K17" s="67">
+      <c r="L17" s="63">
         <f t="shared" si="0"/>
         <v>-11</v>
       </c>
-      <c r="L17" s="72">
+      <c r="M17" s="68">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="M17" s="73" t="s">
+      <c r="N17" s="69" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B18" s="54">
+    <row r="18" spans="2:14" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B18" s="50">
         <v>13</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="78"/>
+      <c r="D18" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="54">
+      <c r="E18" s="50">
         <v>26</v>
       </c>
-      <c r="E18" s="54">
+      <c r="F18" s="50">
         <v>5</v>
       </c>
-      <c r="F18" s="54">
+      <c r="G18" s="50">
         <v>9</v>
       </c>
-      <c r="G18" s="54">
+      <c r="H18" s="50">
         <v>12</v>
       </c>
-      <c r="H18" s="56">
+      <c r="I18" s="52">
         <v>35</v>
       </c>
-      <c r="I18" s="57" t="s">
+      <c r="J18" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="J18" s="58">
+      <c r="K18" s="54">
         <v>50</v>
       </c>
-      <c r="K18" s="54">
+      <c r="L18" s="50">
         <f t="shared" si="0"/>
         <v>-15</v>
       </c>
-      <c r="L18" s="59">
+      <c r="M18" s="55">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="M18" s="19" t="s">
+      <c r="N18" s="82" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B19" s="20">
+    <row r="19" spans="2:14" s="2" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="B19" s="17">
         <v>14</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="79"/>
+      <c r="D19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="20">
+      <c r="E19" s="17">
         <v>26</v>
       </c>
-      <c r="E19" s="20">
+      <c r="F19" s="17">
         <v>3</v>
       </c>
-      <c r="F19" s="20">
+      <c r="G19" s="17">
         <v>5</v>
       </c>
-      <c r="G19" s="20">
+      <c r="H19" s="17">
         <v>18</v>
       </c>
-      <c r="H19" s="22">
+      <c r="I19" s="19">
         <v>25</v>
       </c>
-      <c r="I19" s="23" t="s">
+      <c r="J19" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="J19" s="24">
+      <c r="K19" s="21">
         <v>62</v>
       </c>
-      <c r="K19" s="20">
+      <c r="L19" s="17">
         <f t="shared" si="0"/>
         <v>-37</v>
       </c>
-      <c r="L19" s="25">
+      <c r="M19" s="22">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="M19" s="18"/>
+      <c r="N19" s="83"/>
     </row>
-    <row r="20" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="20" spans="2:14" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B20" s="10"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="9"/>
       <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="2:13" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="2:14" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
       <c r="B21" s="10"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="6"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="9"/>
       <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="M7:M9"/>
-    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="N18:N19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated icons in Allsvenskan2001.xlsx
</commit_message>
<xml_diff>
--- a/EPPlus.WebSampleMvc.NetCore/data/Allsvenskan2001.xlsx
+++ b/EPPlus.WebSampleMvc.NetCore/data/Allsvenskan2001.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mats\dev\EPPlusSoftware\EPPlus.WebSamples\EPPlus.WebSampleMvc.NetCore\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatsAlm\dev\EPPlusSoftware\EPPlus.WebSamples\EPPlus.WebSampleMvc.NetCore\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865597EE-B505-408A-B720-1F4F7B27A8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29431889-156E-4C7E-A2D2-B005D9EA3033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="95880" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CC10EFD2-A4CF-4F7B-8E25-A2032FB846DE}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{CC10EFD2-A4CF-4F7B-8E25-A2032FB846DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -821,815 +821,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>49531</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>352425</xdr:rowOff>
+      <xdr:rowOff>342901</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>259080</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>609600</xdr:rowOff>
+      <xdr:rowOff>552450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A474E74B-40F8-480A-BDB2-C973073F76B8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="866775" y="1657350"/>
-          <a:ext cx="257175" cy="257175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>295276</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{685320DD-2012-4752-AB98-1A73338E66D4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="885826" y="2276476"/>
-          <a:ext cx="228600" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>304801</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8490777C-67E5-4BC6-A743-DE90339D0620}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="876301" y="2533651"/>
-          <a:ext cx="247650" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B9EA950-972F-4E04-8855-5AA5BE8A34C4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="895350" y="2800350"/>
-          <a:ext cx="219075" cy="219075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>323850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>533400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{119B6688-58AA-4A75-8544-C5F5F4F4DE10}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="904875" y="3333750"/>
-          <a:ext cx="209550" cy="209550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85726</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>247651</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AA34F0F-D8CC-4C50-A783-B084A8974154}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="904876" y="4105276"/>
-          <a:ext cx="228600" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8063D6F-D000-43C3-97EF-A5E3E88AE2B1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="904875" y="4381500"/>
-          <a:ext cx="228600" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71DFADCF-FBFE-4A98-BE14-FE420E625E74}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="895350" y="4657725"/>
-          <a:ext cx="238125" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BC702A6-2941-47ED-9916-19C2CEA180D2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="904875" y="4905375"/>
-          <a:ext cx="228600" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD51C384-F21C-46F9-8BD9-E125D89747C0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="904875" y="5143500"/>
-          <a:ext cx="219075" cy="219075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>419100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D54F14BB-3B5E-4B6C-A733-40664626BB72}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="904875" y="5553075"/>
-          <a:ext cx="238125" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E824AA7C-31F2-4BDB-9F21-F478E9D4CB2E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="895350" y="5972175"/>
-          <a:ext cx="257175" cy="257175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE45C00-86C8-433F-8473-019B6793BA4B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="904875" y="6238875"/>
-          <a:ext cx="228600" cy="228600"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84769677-7E2B-4606-AA34-B2812F9E5B9C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85009636-FCE0-4E8E-86CE-957442FD37C4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1638,7 +845,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1651,8 +858,258 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="904875" y="3886200"/>
-          <a:ext cx="200025" cy="200025"/>
+          <a:off x="899161" y="1600201"/>
+          <a:ext cx="209549" cy="209549"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>64771</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{925E6901-894B-4377-A51F-A39E1026B881}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914401" y="2209801"/>
+          <a:ext cx="190499" cy="190499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>68581</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>26671</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>213360</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E612E265-5C0B-4DED-81D1-6C52FC85D435}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="918211" y="2449831"/>
+          <a:ext cx="186689" cy="186689"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>224790</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>228219</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D75D815-79EC-4CE6-8AFD-054AFD48924E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="941070" y="5855970"/>
+          <a:ext cx="133350" cy="178689"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>216789</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7521B80E-C8EE-430E-800B-36152C8E408C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="944880" y="6096000"/>
+          <a:ext cx="133350" cy="178689"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>278131</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>403861</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA77E2AF-F486-4470-A498-AB6038160641}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="880110" y="5410200"/>
+          <a:ext cx="247651" cy="247651"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1963,42 +1420,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047A5EC2-D577-486C-8E0D-C6229686D238}">
   <dimension ref="B1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" customWidth="1"/>
-    <col min="2" max="3" width="5.2265625" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="7" width="5.6796875" customWidth="1"/>
-    <col min="8" max="8" width="5.7265625" customWidth="1"/>
-    <col min="9" max="9" width="3.86328125" customWidth="1"/>
-    <col min="10" max="10" width="2.1796875" customWidth="1"/>
-    <col min="11" max="11" width="3.86328125" customWidth="1"/>
-    <col min="12" max="13" width="5.7265625" customWidth="1"/>
-    <col min="14" max="14" width="13.08984375" customWidth="1"/>
+    <col min="1" max="1" width="6.5234375" customWidth="1"/>
+    <col min="2" max="3" width="5.20703125" customWidth="1"/>
+    <col min="4" max="4" width="18.47265625" customWidth="1"/>
+    <col min="5" max="7" width="5.68359375" customWidth="1"/>
+    <col min="8" max="8" width="5.734375" customWidth="1"/>
+    <col min="9" max="9" width="3.83984375" customWidth="1"/>
+    <col min="10" max="10" width="2.15625" customWidth="1"/>
+    <col min="11" max="11" width="3.83984375" customWidth="1"/>
+    <col min="12" max="13" width="5.734375" customWidth="1"/>
+    <col min="14" max="14" width="13.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="21" x14ac:dyDescent="1">
+    <row r="1" spans="2:22" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.75">
+    <row r="3" spans="2:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="21.75" thickBot="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="4" spans="2:22" ht="20.7" thickBot="1" x14ac:dyDescent="0.8">
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:22" s="2" customFormat="1" ht="30.25" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="5" spans="2:22" s="2" customFormat="1" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B5" s="23"/>
       <c r="C5" s="70"/>
       <c r="D5" s="24" t="s">
@@ -2032,7 +1489,7 @@
       </c>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="2:22" s="2" customFormat="1" ht="73.75" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:22" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="56">
         <v>1</v>
       </c>
@@ -2076,7 +1533,7 @@
       <c r="R6"/>
       <c r="S6"/>
     </row>
-    <row r="7" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="2:22" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="26">
         <v>2</v>
       </c>
@@ -2119,7 +1576,7 @@
       <c r="S7"/>
       <c r="T7"/>
     </row>
-    <row r="8" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="8" spans="2:22" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="32">
         <v>3</v>
       </c>
@@ -2158,7 +1615,7 @@
       </c>
       <c r="N8" s="81"/>
     </row>
-    <row r="9" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="9" spans="2:22" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="32">
         <v>4</v>
       </c>
@@ -2197,7 +1654,7 @@
       </c>
       <c r="N9" s="81"/>
     </row>
-    <row r="10" spans="2:22" s="2" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="10" spans="2:22" s="2" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="38">
         <v>5</v>
       </c>
@@ -2240,7 +1697,7 @@
       <c r="R10"/>
       <c r="V10"/>
     </row>
-    <row r="11" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="11" spans="2:22" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="44">
         <v>6</v>
       </c>
@@ -2279,7 +1736,7 @@
       </c>
       <c r="N11" s="15"/>
     </row>
-    <row r="12" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="12" spans="2:22" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="44">
         <v>7</v>
       </c>
@@ -2318,7 +1775,7 @@
       </c>
       <c r="N12" s="15"/>
     </row>
-    <row r="13" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="2:22" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="44">
         <v>8</v>
       </c>
@@ -2357,7 +1814,7 @@
       </c>
       <c r="N13" s="15"/>
     </row>
-    <row r="14" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="2:22" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="44">
         <v>9</v>
       </c>
@@ -2396,7 +1853,7 @@
       </c>
       <c r="N14" s="15"/>
     </row>
-    <row r="15" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="15" spans="2:22" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="44">
         <v>10</v>
       </c>
@@ -2435,7 +1892,7 @@
       </c>
       <c r="N15" s="15"/>
     </row>
-    <row r="16" spans="2:22" s="2" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="16" spans="2:22" s="2" customFormat="1" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B16" s="3">
         <v>11</v>
       </c>
@@ -2474,7 +1931,7 @@
       </c>
       <c r="N16" s="15"/>
     </row>
-    <row r="17" spans="2:14" s="2" customFormat="1" ht="45" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="2:14" s="2" customFormat="1" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B17" s="63">
         <v>12</v>
       </c>
@@ -2515,7 +1972,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:14" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="18" spans="2:14" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="50">
         <v>13</v>
       </c>
@@ -2556,7 +2013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:14" s="2" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="19" spans="2:14" s="2" customFormat="1" ht="20.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="B19" s="17">
         <v>14</v>
       </c>
@@ -2595,7 +2052,7 @@
       </c>
       <c r="N19" s="83"/>
     </row>
-    <row r="20" spans="2:14" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="20" spans="2:14" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="6"/>
@@ -2609,7 +2066,7 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="2:14" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="21" spans="2:14" s="2" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="6"/>

</xml_diff>